<commit_message>
adds R files Misja
</commit_message>
<xml_diff>
--- a/source/football.xlsx
+++ b/source/football.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/misja/stack/Research/Cursus/Football/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcmik\stack\Misja\lesgeven\NZa datascience\inlezen data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="28800" windowHeight="16500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Points" sheetId="1" r:id="rId1"/>
@@ -17,9 +17,6 @@
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -140,13 +137,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Stand." xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -418,17 +418,17 @@
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="A4" sqref="A4:B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -436,7 +436,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -444,7 +444,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -452,7 +452,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -460,7 +460,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -468,7 +468,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -476,7 +476,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -484,7 +484,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -492,7 +492,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -500,7 +500,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -508,7 +508,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -516,7 +516,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -524,7 +524,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -532,7 +532,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -540,7 +540,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -548,7 +548,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -556,7 +556,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -564,7 +564,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -572,7 +572,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -613,17 +613,17 @@
       <selection activeCell="A5" sqref="A5:A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -631,7 +631,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -639,7 +639,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -647,7 +647,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -655,7 +655,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -663,7 +663,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -671,7 +671,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -679,7 +679,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -687,7 +687,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -695,7 +695,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -703,7 +703,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -711,7 +711,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -719,7 +719,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -727,7 +727,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -735,7 +735,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -743,7 +743,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -751,7 +751,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -759,7 +759,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -767,7 +767,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>21</v>
       </c>

</xml_diff>